<commit_message>
Teste do Junit contruido e funcionando.
</commit_message>
<xml_diff>
--- a/docs/Analise Valor Limite.xlsx
+++ b/docs/Analise Valor Limite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charleston Campos\git\ProjetoSpring\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charleston\git\ProjetoSpring\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
   <si>
     <t>Analise do Valor Limite - Método: salvarCliente</t>
   </si>
@@ -60,21 +60,12 @@
     <t xml:space="preserve"> -</t>
   </si>
   <si>
-    <t>Preencha o CPF do Cliente</t>
-  </si>
-  <si>
     <t>336.211.075-41</t>
   </si>
   <si>
-    <t>Preencha o E-mail do Cliente</t>
-  </si>
-  <si>
     <t>charlinhocjc@gmail.com</t>
   </si>
   <si>
-    <t>Preencha o Nome do Cliente</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NULL</t>
   </si>
   <si>
@@ -84,18 +75,12 @@
     <t>Objeto Endereço</t>
   </si>
   <si>
-    <t>Faixa Salarial não foi informada!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Objeto Renda </t>
   </si>
   <si>
     <t>cliente.getSenha</t>
   </si>
   <si>
-    <t>Preencha a Senha do Cliente</t>
-  </si>
-  <si>
     <t>Pobre</t>
   </si>
   <si>
@@ -114,20 +99,20 @@
     <t>Classe Alta</t>
   </si>
   <si>
-    <t>Favor preencha o Endereço corretamente!</t>
-  </si>
-  <si>
     <t>TOTAL: 12</t>
   </si>
   <si>
     <t>Analise do Valor Limite - Método: efetuarLogin</t>
+  </si>
+  <si>
+    <t>cliente/falha-cadastrar-cliente.jsp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +140,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,13 +210,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -233,6 +223,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -517,7 +511,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,45 +528,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="2"/>
@@ -601,13 +595,13 @@
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>123456</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -629,17 +623,17 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>123456</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -657,23 +651,23 @@
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>123456</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
@@ -685,23 +679,23 @@
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>123456</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
@@ -713,26 +707,26 @@
         <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>123456</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
@@ -741,175 +735,175 @@
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>123456</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1">
         <v>700</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>23</v>
+      <c r="H9" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>123456</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G10" s="1">
         <v>1540</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>123456</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G11" s="1">
         <v>1925</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>123456</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G12" s="1">
         <v>2813</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>123456</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G13" s="1">
         <v>4845</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>123456</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G14" s="1">
         <v>12988</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -927,8 +921,8 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>30</v>
+      <c r="A16" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1082,26 +1076,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1114,7 +1108,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1124,7 +1118,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1134,9 +1128,9 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1144,9 +1138,9 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1154,9 +1148,9 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1164,9 +1158,9 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="8"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1174,9 +1168,9 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1184,9 +1178,9 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1194,9 +1188,9 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1204,9 +1198,9 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1214,9 +1208,9 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="8"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>

</xml_diff>

<commit_message>
Implementação da interface DAO e criação da tabela do valor limite do metodo efetuarLogin.
</commit_message>
<xml_diff>
--- a/docs/Analise Valor Limite.xlsx
+++ b/docs/Analise Valor Limite.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charleston\git\ProjetoSpring\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ProjetoSpring\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SalvarCliente" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
   <si>
     <t>Analise do Valor Limite - Método: salvarCliente</t>
   </si>
@@ -106,6 +106,42 @@
   </si>
   <si>
     <t>cliente/falha-cadastrar-cliente.jsp</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>listaItens</t>
+  </si>
+  <si>
+    <t>resultados</t>
+  </si>
+  <si>
+    <t>cliente valido</t>
+  </si>
+  <si>
+    <t>1  tem</t>
+  </si>
+  <si>
+    <t>redirect:/listaProdutosCarrinho</t>
+  </si>
+  <si>
+    <t>cliente invalido</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>cliente/falha-login-cliente</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - </t>
   </si>
 </sst>
 </file>
@@ -210,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -223,10 +259,38 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -510,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -528,16 +592,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
       <c r="I1" s="6"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -762,7 +826,7 @@
       <c r="G9" s="1">
         <v>700</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J9" s="2"/>
@@ -1066,161 +1130,191 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
+      <c r="A2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="A3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="A4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="A5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="A6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Concluido o teste do metodo salvarCliente.
</commit_message>
<xml_diff>
--- a/docs/Analise Valor Limite.xlsx
+++ b/docs/Analise Valor Limite.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ProjetoSpring\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charleston\git\ProjetoSpring\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="SalvarCliente" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
   <si>
     <t>Analise do Valor Limite - Método: salvarCliente</t>
   </si>
@@ -81,33 +81,12 @@
     <t>cliente.getSenha</t>
   </si>
   <si>
-    <t>Pobre</t>
-  </si>
-  <si>
-    <t>Classe Media Baixa</t>
-  </si>
-  <si>
-    <t>Classe Media</t>
-  </si>
-  <si>
-    <t>Classe Media Alta</t>
-  </si>
-  <si>
-    <t>Classe Alta Baixa</t>
-  </si>
-  <si>
-    <t>Classe Alta</t>
-  </si>
-  <si>
     <t>TOTAL: 12</t>
   </si>
   <si>
     <t>Analise do Valor Limite - Método: efetuarLogin</t>
   </si>
   <si>
-    <t>cliente/falha-cadastrar-cliente.jsp</t>
-  </si>
-  <si>
     <t>Cliente</t>
   </si>
   <si>
@@ -142,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">        - </t>
+  </si>
+  <si>
+    <t>cliente/falha-cadastrar-cliente</t>
+  </si>
+  <si>
+    <t>cliente/sucesso-cadastro-cliente</t>
   </si>
 </sst>
 </file>
@@ -260,9 +245,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -291,6 +273,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -574,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,16 +577,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="6"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -659,7 +644,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -687,7 +672,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -715,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -743,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -771,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -799,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -827,7 +812,7 @@
         <v>700</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -855,7 +840,7 @@
         <v>1540</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -883,7 +868,7 @@
         <v>1925</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -911,7 +896,7 @@
         <v>2813</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -939,7 +924,7 @@
         <v>4845</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -967,7 +952,7 @@
         <v>12988</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -986,7 +971,7 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1130,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1142,11 +1127,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="A1" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1154,30 +1139,30 @@
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="A2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>32</v>
+      <c r="A3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1186,14 +1171,14 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>34</v>
+      <c r="A4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1202,14 +1187,14 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>34</v>
+      <c r="C5" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1218,14 +1203,14 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>35</v>
+      <c r="A6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1234,9 +1219,9 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1244,9 +1229,9 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1254,9 +1239,9 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1264,9 +1249,9 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1274,9 +1259,9 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1284,9 +1269,9 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1294,9 +1279,9 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1304,9 +1289,9 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>

</xml_diff>

<commit_message>
Implementação da classe TesteLogin.java
</commit_message>
<xml_diff>
--- a/docs/Analise Valor Limite.xlsx
+++ b/docs/Analise Valor Limite.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charleston\git\ProjetoSpring\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ProjetoSpring\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SalvarCliente" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="33">
   <si>
     <t>Analise do Valor Limite - Método: salvarCliente</t>
   </si>
@@ -102,18 +102,9 @@
     <t>1  tem</t>
   </si>
   <si>
-    <t>redirect:/listaProdutosCarrinho</t>
-  </si>
-  <si>
     <t>cliente invalido</t>
   </si>
   <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>cliente/falha-login-cliente</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -127,6 +118,12 @@
   </si>
   <si>
     <t>cliente/sucesso-cadastro-cliente</t>
+  </si>
+  <si>
+    <t>Olá, Fulano de Tal</t>
+  </si>
+  <si>
+    <t>Usuário ou Senha Invalidos!</t>
   </si>
 </sst>
 </file>
@@ -559,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -644,7 +641,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -672,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -700,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -728,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -756,7 +753,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -784,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -812,7 +809,7 @@
         <v>700</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -840,7 +837,7 @@
         <v>1540</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -868,7 +865,7 @@
         <v>1925</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -896,7 +893,7 @@
         <v>2813</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -924,7 +921,7 @@
         <v>4845</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -952,7 +949,7 @@
         <v>12988</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1115,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1159,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1175,10 +1172,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1191,10 +1188,10 @@
         <v>23</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1204,13 +1201,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>

</xml_diff>